<commit_message>
rewrite part of search, add new data
</commit_message>
<xml_diff>
--- a/data-migration/xlsx_1900-/1901_Sommer.xlsx
+++ b/data-migration/xlsx_1900-/1901_Sommer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TEMP REPOSITORY\VVZ 1833-2014\_XLSX_2024-05-22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\TEMP REPOSITORY\VVZ 1833-2014\_XLSX_2024-05-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D0817C-EDD1-4705-B20C-10CB978AD14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917ACE71-6B9C-42F8-BB69-64B10FCFEF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="1023">
   <si>
     <t>1901</t>
   </si>
@@ -2898,9 +2898,6 @@
     <t>haab_o</t>
   </si>
   <si>
-    <t>fick_ae</t>
-  </si>
-  <si>
     <t>wyder_t</t>
   </si>
   <si>
@@ -2988,9 +2985,6 @@
     <t>betz_lp</t>
   </si>
   <si>
-    <t>meyervonknonau_g</t>
-  </si>
-  <si>
     <t>billeter_g</t>
   </si>
   <si>
@@ -3060,9 +3054,6 @@
     <t>overton_e</t>
   </si>
   <si>
-    <t>schinz_h1</t>
-  </si>
-  <si>
     <t>kuendig_j</t>
   </si>
   <si>
@@ -3100,6 +3091,18 @@
   </si>
   <si>
     <t>heim_a1</t>
+  </si>
+  <si>
+    <t>fick_age</t>
+  </si>
+  <si>
+    <t>meyer-knonau_g</t>
+  </si>
+  <si>
+    <t>schinz_h</t>
+  </si>
+  <si>
+    <t>HP</t>
   </si>
 </sst>
 </file>
@@ -3452,21 +3455,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F268" workbookViewId="0">
-      <selection activeCell="H296" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G74" workbookViewId="0">
+      <selection activeCell="L96" sqref="L96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="30.54296875" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="123" customWidth="1"/>
-    <col min="7" max="7" width="55.90625" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3495,7 +3498,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3524,7 +3527,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3579,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -3628,7 +3631,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3784,7 +3787,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -3810,7 +3813,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -3836,7 +3839,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -3865,7 +3868,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -3923,7 +3926,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -3952,7 +3955,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3978,7 +3981,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -4004,7 +4007,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -4082,7 +4085,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -4160,7 +4163,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4215,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -4238,7 +4241,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -4264,7 +4267,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -4287,10 +4290,10 @@
         <v>908</v>
       </c>
       <c r="I31" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -4316,7 +4319,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -4342,7 +4345,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -4368,7 +4371,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -4394,7 +4397,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -4420,7 +4423,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -4446,7 +4449,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -4472,7 +4475,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -4498,7 +4501,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -4550,7 +4553,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -4576,7 +4579,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -4602,7 +4605,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -4628,7 +4631,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -4654,7 +4657,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -4680,7 +4683,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -4706,7 +4709,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4738,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -4761,7 +4764,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -4787,7 +4790,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -4842,7 +4845,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -4871,7 +4874,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -4897,7 +4900,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -5001,7 +5004,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -5027,7 +5030,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -5053,7 +5056,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -5079,7 +5082,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -5105,7 +5108,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -5131,7 +5134,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -5157,7 +5160,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -5183,7 +5186,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -5212,7 +5215,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -5247,7 +5250,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -5270,7 +5273,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -5305,7 +5308,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -5346,7 +5349,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -5372,7 +5375,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -5398,7 +5401,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -5424,7 +5427,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -5450,7 +5453,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -5476,7 +5479,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -5502,7 +5505,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -5528,7 +5531,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -5554,7 +5557,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -5580,7 +5583,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -5606,7 +5609,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -5632,7 +5635,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -5658,7 +5661,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -5684,7 +5687,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -5710,7 +5713,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -5736,7 +5739,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -5788,7 +5791,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +5817,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -5840,7 +5843,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -5866,7 +5869,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -5892,7 +5895,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -5918,7 +5921,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -5963,11 +5966,11 @@
       <c r="G94" t="s">
         <v>4</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -5986,11 +5989,11 @@
       <c r="G95" t="s">
         <v>133</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -6009,11 +6012,11 @@
       <c r="G96" t="s">
         <v>845</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -6032,11 +6035,11 @@
       <c r="G97" t="s">
         <v>656</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -6062,7 +6065,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -6114,7 +6117,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -6140,7 +6143,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -6192,7 +6195,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -6218,7 +6221,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -6270,7 +6273,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -6296,7 +6299,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -6322,7 +6325,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -6348,7 +6351,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -6374,7 +6377,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -6400,7 +6403,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6429,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -6452,7 +6455,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -6478,7 +6481,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -6504,7 +6507,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -6530,7 +6533,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -6556,7 +6559,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -6582,7 +6585,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -6608,7 +6611,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -6634,7 +6637,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -6660,7 +6663,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -6686,7 +6689,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -6712,7 +6715,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -6738,7 +6741,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -6764,7 +6767,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -6790,7 +6793,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -6816,7 +6819,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -6842,7 +6845,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -6868,7 +6871,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -6894,7 +6897,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -6920,7 +6923,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -6946,7 +6949,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -6972,7 +6975,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -6998,7 +7001,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -7024,7 +7027,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -7044,13 +7047,13 @@
         <v>303</v>
       </c>
       <c r="H136" t="s">
-        <v>954</v>
+        <v>1019</v>
       </c>
       <c r="I136" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -7070,13 +7073,13 @@
         <v>875</v>
       </c>
       <c r="H137" t="s">
-        <v>954</v>
+        <v>1019</v>
       </c>
       <c r="I137" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -7096,13 +7099,13 @@
         <v>878</v>
       </c>
       <c r="H138" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I138" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -7122,13 +7125,13 @@
         <v>352</v>
       </c>
       <c r="H139" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I139" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -7148,13 +7151,13 @@
         <v>164</v>
       </c>
       <c r="H140" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I140" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -7174,13 +7177,13 @@
         <v>356</v>
       </c>
       <c r="H141" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I141" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -7200,13 +7203,13 @@
         <v>34</v>
       </c>
       <c r="H142" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I142" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -7226,13 +7229,13 @@
         <v>361</v>
       </c>
       <c r="H143" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I143" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -7252,13 +7255,13 @@
         <v>4</v>
       </c>
       <c r="H144" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I144" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -7278,13 +7281,13 @@
         <v>366</v>
       </c>
       <c r="H145" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I145" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -7304,13 +7307,13 @@
         <v>369</v>
       </c>
       <c r="H146" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I146" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -7330,13 +7333,13 @@
         <v>372</v>
       </c>
       <c r="H147" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I147" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -7356,13 +7359,13 @@
         <v>375</v>
       </c>
       <c r="H148" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I148" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -7382,13 +7385,13 @@
         <v>378</v>
       </c>
       <c r="H149" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I149" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -7408,13 +7411,13 @@
         <v>381</v>
       </c>
       <c r="H150" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I150" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -7434,13 +7437,13 @@
         <v>384</v>
       </c>
       <c r="H151" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I151" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -7460,13 +7463,13 @@
         <v>387</v>
       </c>
       <c r="H152" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I152" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -7486,13 +7489,13 @@
         <v>390</v>
       </c>
       <c r="H153" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I153" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -7512,13 +7515,13 @@
         <v>393</v>
       </c>
       <c r="H154" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I154" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -7538,13 +7541,13 @@
         <v>395</v>
       </c>
       <c r="H155" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I155" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -7564,13 +7567,13 @@
         <v>395</v>
       </c>
       <c r="H156" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I156" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -7590,13 +7593,13 @@
         <v>398</v>
       </c>
       <c r="H157" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I157" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -7616,13 +7619,13 @@
         <v>400</v>
       </c>
       <c r="H158" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I158" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -7642,13 +7645,13 @@
         <v>403</v>
       </c>
       <c r="H159" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I159" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -7668,13 +7671,13 @@
         <v>406</v>
       </c>
       <c r="H160" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I160" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -7694,13 +7697,13 @@
         <v>409</v>
       </c>
       <c r="H161" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I161" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -7720,13 +7723,13 @@
         <v>412</v>
       </c>
       <c r="H162" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I162" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -7746,13 +7749,13 @@
         <v>261</v>
       </c>
       <c r="H163" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I163" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -7772,13 +7775,13 @@
         <v>417</v>
       </c>
       <c r="H164" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I164" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -7798,13 +7801,13 @@
         <v>261</v>
       </c>
       <c r="H165" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I165" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -7824,13 +7827,13 @@
         <v>422</v>
       </c>
       <c r="H166" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I166" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -7850,13 +7853,13 @@
         <v>425</v>
       </c>
       <c r="H167" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I167" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -7876,13 +7879,13 @@
         <v>428</v>
       </c>
       <c r="H168" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I168" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -7902,13 +7905,13 @@
         <v>431</v>
       </c>
       <c r="H169" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I169" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -7928,13 +7931,13 @@
         <v>272</v>
       </c>
       <c r="H170" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I170" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -7954,13 +7957,13 @@
         <v>436</v>
       </c>
       <c r="H171" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I171" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -7980,13 +7983,13 @@
         <v>439</v>
       </c>
       <c r="H172" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I172" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -8006,13 +8009,13 @@
         <v>442</v>
       </c>
       <c r="H173" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I173" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -8032,13 +8035,13 @@
         <v>445</v>
       </c>
       <c r="H174" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I174" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -8058,13 +8061,13 @@
         <v>4</v>
       </c>
       <c r="H175" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I175" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -8084,13 +8087,13 @@
         <v>4</v>
       </c>
       <c r="H176" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I176" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -8116,7 +8119,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -8142,7 +8145,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -8162,13 +8165,13 @@
         <v>457</v>
       </c>
       <c r="H179" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I179" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>0</v>
       </c>
@@ -8188,13 +8191,13 @@
         <v>460</v>
       </c>
       <c r="H180" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I180" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -8214,13 +8217,13 @@
         <v>463</v>
       </c>
       <c r="H181" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I181" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -8240,13 +8243,13 @@
         <v>466</v>
       </c>
       <c r="H182" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I182" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -8266,13 +8269,13 @@
         <v>34</v>
       </c>
       <c r="H183" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I183" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -8292,13 +8295,13 @@
         <v>471</v>
       </c>
       <c r="H184" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I184" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -8318,13 +8321,13 @@
         <v>4</v>
       </c>
       <c r="H185" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I185" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -8344,13 +8347,13 @@
         <v>476</v>
       </c>
       <c r="H186" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I186" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -8370,13 +8373,13 @@
         <v>261</v>
       </c>
       <c r="H187" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I187" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -8396,13 +8399,13 @@
         <v>481</v>
       </c>
       <c r="H188" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I188" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -8422,13 +8425,13 @@
         <v>7</v>
       </c>
       <c r="H189" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I189" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -8448,13 +8451,13 @@
         <v>486</v>
       </c>
       <c r="H190" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I190" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -8474,13 +8477,13 @@
         <v>7</v>
       </c>
       <c r="H191" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I191" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -8500,13 +8503,13 @@
         <v>490</v>
       </c>
       <c r="H192" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I192" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -8526,13 +8529,13 @@
         <v>493</v>
       </c>
       <c r="H193" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I193" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>0</v>
       </c>
@@ -8552,13 +8555,13 @@
         <v>496</v>
       </c>
       <c r="H194" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I194" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>0</v>
       </c>
@@ -8578,13 +8581,13 @@
         <v>48</v>
       </c>
       <c r="H195" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I195" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -8604,13 +8607,13 @@
         <v>501</v>
       </c>
       <c r="H196" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I196" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -8630,13 +8633,13 @@
         <v>504</v>
       </c>
       <c r="H197" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I197" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -8656,13 +8659,13 @@
         <v>507</v>
       </c>
       <c r="H198" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I198" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>0</v>
       </c>
@@ -8682,13 +8685,13 @@
         <v>510</v>
       </c>
       <c r="H199" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I199" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -8708,13 +8711,13 @@
         <v>513</v>
       </c>
       <c r="H200" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I200" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -8734,13 +8737,13 @@
         <v>516</v>
       </c>
       <c r="H201" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I201" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -8760,13 +8763,13 @@
         <v>261</v>
       </c>
       <c r="H202" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I202" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -8786,13 +8789,13 @@
         <v>98</v>
       </c>
       <c r="H203" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I203" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -8812,13 +8815,13 @@
         <v>523</v>
       </c>
       <c r="H204" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I204" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -8838,13 +8841,13 @@
         <v>526</v>
       </c>
       <c r="H205" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I205" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -8864,13 +8867,13 @@
         <v>529</v>
       </c>
       <c r="H206" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I206" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -8890,13 +8893,13 @@
         <v>531</v>
       </c>
       <c r="H207" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I207" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>0</v>
       </c>
@@ -8916,13 +8919,13 @@
         <v>534</v>
       </c>
       <c r="H208" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I208" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -8942,13 +8945,13 @@
         <v>537</v>
       </c>
       <c r="H209" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I209" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -8968,13 +8971,13 @@
         <v>539</v>
       </c>
       <c r="H210" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I210" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -8994,13 +8997,13 @@
         <v>542</v>
       </c>
       <c r="H211" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I211" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>0</v>
       </c>
@@ -9020,13 +9023,13 @@
         <v>436</v>
       </c>
       <c r="H212" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I212" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -9046,13 +9049,13 @@
         <v>547</v>
       </c>
       <c r="H213" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I213" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>0</v>
       </c>
@@ -9072,13 +9075,13 @@
         <v>550</v>
       </c>
       <c r="H214" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I214" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>0</v>
       </c>
@@ -9098,13 +9101,13 @@
         <v>553</v>
       </c>
       <c r="H215" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I215" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>0</v>
       </c>
@@ -9124,13 +9127,13 @@
         <v>25</v>
       </c>
       <c r="H216" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I216" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -9150,13 +9153,13 @@
         <v>557</v>
       </c>
       <c r="H217" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I217" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>0</v>
       </c>
@@ -9176,13 +9179,13 @@
         <v>31</v>
       </c>
       <c r="H218" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I218" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>0</v>
       </c>
@@ -9202,13 +9205,13 @@
         <v>133</v>
       </c>
       <c r="H219" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I219" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>0</v>
       </c>
@@ -9228,13 +9231,13 @@
         <v>563</v>
       </c>
       <c r="H220" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I220" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>0</v>
       </c>
@@ -9254,13 +9257,13 @@
         <v>4</v>
       </c>
       <c r="H221" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I221" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -9280,13 +9283,13 @@
         <v>568</v>
       </c>
       <c r="H222" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I222" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -9306,13 +9309,13 @@
         <v>571</v>
       </c>
       <c r="H223" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I223" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -9332,13 +9335,13 @@
         <v>164</v>
       </c>
       <c r="H224" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I224" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -9358,13 +9361,13 @@
         <v>576</v>
       </c>
       <c r="H225" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I225" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -9384,13 +9387,13 @@
         <v>7</v>
       </c>
       <c r="H226" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I226" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -9410,13 +9413,13 @@
         <v>7</v>
       </c>
       <c r="H227" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I227" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -9436,13 +9439,13 @@
         <v>583</v>
       </c>
       <c r="H228" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I228" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -9462,13 +9465,13 @@
         <v>481</v>
       </c>
       <c r="H229" t="s">
-        <v>984</v>
+        <v>1020</v>
       </c>
       <c r="I229" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -9488,13 +9491,13 @@
         <v>7</v>
       </c>
       <c r="H230" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="I230" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -9514,13 +9517,13 @@
         <v>4</v>
       </c>
       <c r="H231" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="I231" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -9540,13 +9543,13 @@
         <v>591</v>
       </c>
       <c r="H232" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="I232" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -9566,13 +9569,13 @@
         <v>48</v>
       </c>
       <c r="H233" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="I233" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>0</v>
       </c>
@@ -9592,13 +9595,13 @@
         <v>596</v>
       </c>
       <c r="H234" t="s">
-        <v>984</v>
+        <v>1020</v>
       </c>
       <c r="I234" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>0</v>
       </c>
@@ -9618,13 +9621,13 @@
         <v>599</v>
       </c>
       <c r="H235" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="I235" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>0</v>
       </c>
@@ -9644,13 +9647,13 @@
         <v>602</v>
       </c>
       <c r="H236" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="I236" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -9670,13 +9673,13 @@
         <v>605</v>
       </c>
       <c r="H237" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="I237" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>0</v>
       </c>
@@ -9696,7 +9699,7 @@
         <v>608</v>
       </c>
       <c r="H238" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="I238" t="s">
         <v>893</v>
@@ -9705,7 +9708,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>0</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>857</v>
       </c>
       <c r="H239" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="I239" t="s">
         <v>893</v>
@@ -9734,7 +9737,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>0</v>
       </c>
@@ -9754,13 +9757,13 @@
         <v>612</v>
       </c>
       <c r="H240" t="s">
-        <v>984</v>
+        <v>1020</v>
       </c>
       <c r="I240" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>0</v>
       </c>
@@ -9780,13 +9783,13 @@
         <v>614</v>
       </c>
       <c r="H241" t="s">
-        <v>984</v>
+        <v>1020</v>
       </c>
       <c r="I241" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -9806,13 +9809,13 @@
         <v>617</v>
       </c>
       <c r="H242" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="I242" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -9832,13 +9835,13 @@
         <v>620</v>
       </c>
       <c r="H243" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="I243" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -9858,7 +9861,7 @@
         <v>623</v>
       </c>
       <c r="H244" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="I244" t="s">
         <v>893</v>
@@ -9867,7 +9870,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -9887,13 +9890,13 @@
         <v>626</v>
       </c>
       <c r="H245" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="I245" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -9913,13 +9916,13 @@
         <v>884</v>
       </c>
       <c r="H246" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I246" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -9939,13 +9942,13 @@
         <v>48</v>
       </c>
       <c r="H247" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="I247" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -9965,13 +9968,13 @@
         <v>4</v>
       </c>
       <c r="H248" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="I248" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -9991,13 +9994,13 @@
         <v>7</v>
       </c>
       <c r="H249" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="I249" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -10017,13 +10020,13 @@
         <v>103</v>
       </c>
       <c r="H250" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="I250" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -10043,13 +10046,13 @@
         <v>639</v>
       </c>
       <c r="H251" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="I251" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -10069,13 +10072,13 @@
         <v>642</v>
       </c>
       <c r="H252" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="I252" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -10095,13 +10098,13 @@
         <v>645</v>
       </c>
       <c r="H253" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="I253" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>0</v>
       </c>
@@ -10121,13 +10124,13 @@
         <v>648</v>
       </c>
       <c r="H254" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="I254" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -10147,13 +10150,13 @@
         <v>651</v>
       </c>
       <c r="H255" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="I255" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>0</v>
       </c>
@@ -10173,13 +10176,13 @@
         <v>4</v>
       </c>
       <c r="H256" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I256" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -10199,13 +10202,13 @@
         <v>656</v>
       </c>
       <c r="H257" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I257" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -10225,13 +10228,13 @@
         <v>4</v>
       </c>
       <c r="H258" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I258" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>0</v>
       </c>
@@ -10251,13 +10254,13 @@
         <v>48</v>
       </c>
       <c r="H259" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I259" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -10277,13 +10280,13 @@
         <v>4</v>
       </c>
       <c r="H260" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="I260" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>0</v>
       </c>
@@ -10303,13 +10306,13 @@
         <v>656</v>
       </c>
       <c r="H261" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="I261" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -10329,13 +10332,13 @@
         <v>4</v>
       </c>
       <c r="H262" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="I262" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>0</v>
       </c>
@@ -10355,13 +10358,13 @@
         <v>656</v>
       </c>
       <c r="H263" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="I263" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>0</v>
       </c>
@@ -10381,13 +10384,13 @@
         <v>4</v>
       </c>
       <c r="H264" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I264" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>0</v>
       </c>
@@ -10407,13 +10410,13 @@
         <v>37</v>
       </c>
       <c r="H265" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I265" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>0</v>
       </c>
@@ -10433,13 +10436,13 @@
         <v>4</v>
       </c>
       <c r="H266" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I266" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -10462,13 +10465,13 @@
         <v>886</v>
       </c>
       <c r="H267" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="I267" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>0</v>
       </c>
@@ -10488,13 +10491,13 @@
         <v>679</v>
       </c>
       <c r="H268" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="I268" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>0</v>
       </c>
@@ -10517,13 +10520,13 @@
         <v>682</v>
       </c>
       <c r="H269" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="I269" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>0</v>
       </c>
@@ -10543,13 +10546,13 @@
         <v>685</v>
       </c>
       <c r="H270" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I270" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>0</v>
       </c>
@@ -10569,13 +10572,13 @@
         <v>4</v>
       </c>
       <c r="H271" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I271" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>0</v>
       </c>
@@ -10595,13 +10598,13 @@
         <v>690</v>
       </c>
       <c r="H272" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I272" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>0</v>
       </c>
@@ -10621,13 +10624,13 @@
         <v>185</v>
       </c>
       <c r="H273" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="I273" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>0</v>
       </c>
@@ -10647,13 +10650,13 @@
         <v>44</v>
       </c>
       <c r="H274" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I274" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>0</v>
       </c>
@@ -10673,13 +10676,13 @@
         <v>22</v>
       </c>
       <c r="H275" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I275" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>0</v>
       </c>
@@ -10699,13 +10702,13 @@
         <v>185</v>
       </c>
       <c r="H276" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I276" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>0</v>
       </c>
@@ -10725,13 +10728,13 @@
         <v>185</v>
       </c>
       <c r="H277" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I277" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>0</v>
       </c>
@@ -10751,13 +10754,13 @@
         <v>869</v>
       </c>
       <c r="H278" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I278" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>0</v>
       </c>
@@ -10777,13 +10780,13 @@
         <v>869</v>
       </c>
       <c r="H279" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I279" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>0</v>
       </c>
@@ -10803,13 +10806,13 @@
         <v>704</v>
       </c>
       <c r="H280" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I280" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>0</v>
       </c>
@@ -10829,13 +10832,13 @@
         <v>707</v>
       </c>
       <c r="H281" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I281" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>0</v>
       </c>
@@ -10855,13 +10858,13 @@
         <v>710</v>
       </c>
       <c r="H282" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I282" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>0</v>
       </c>
@@ -10881,13 +10884,13 @@
         <v>713</v>
       </c>
       <c r="H283" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I283" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>0</v>
       </c>
@@ -10907,13 +10910,13 @@
         <v>716</v>
       </c>
       <c r="H284" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I284" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>0</v>
       </c>
@@ -10933,13 +10936,13 @@
         <v>719</v>
       </c>
       <c r="H285" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I285" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>0</v>
       </c>
@@ -10959,13 +10962,13 @@
         <v>722</v>
       </c>
       <c r="H286" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I286" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>0</v>
       </c>
@@ -10985,13 +10988,13 @@
         <v>866</v>
       </c>
       <c r="H287" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I287" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>0</v>
       </c>
@@ -11011,13 +11014,13 @@
         <v>185</v>
       </c>
       <c r="H288" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I288" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>0</v>
       </c>
@@ -11037,13 +11040,13 @@
         <v>728</v>
       </c>
       <c r="H289" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I289" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>0</v>
       </c>
@@ -11063,13 +11066,13 @@
         <v>48</v>
       </c>
       <c r="H290" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I290" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>0</v>
       </c>
@@ -11089,13 +11092,13 @@
         <v>7</v>
       </c>
       <c r="H291" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I291" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>0</v>
       </c>
@@ -11118,13 +11121,13 @@
         <v>735</v>
       </c>
       <c r="H292" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I292" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>0</v>
       </c>
@@ -11147,13 +11150,13 @@
         <v>48</v>
       </c>
       <c r="H293" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I293" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>0</v>
       </c>
@@ -11176,13 +11179,13 @@
         <v>34</v>
       </c>
       <c r="H294" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I294" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>0</v>
       </c>
@@ -11205,13 +11208,13 @@
         <v>185</v>
       </c>
       <c r="H295" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I295" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>0</v>
       </c>
@@ -11231,13 +11234,13 @@
         <v>744</v>
       </c>
       <c r="H296" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="I296" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>0</v>
       </c>
@@ -11257,13 +11260,13 @@
         <v>4</v>
       </c>
       <c r="H297" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="I297" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>0</v>
       </c>
@@ -11283,13 +11286,13 @@
         <v>749</v>
       </c>
       <c r="H298" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="I298" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>0</v>
       </c>
@@ -11312,13 +11315,13 @@
         <v>48</v>
       </c>
       <c r="H299" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="I299" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>0</v>
       </c>
@@ -11338,13 +11341,13 @@
         <v>4</v>
       </c>
       <c r="H300" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I300" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>0</v>
       </c>
@@ -11364,13 +11367,13 @@
         <v>4</v>
       </c>
       <c r="H301" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I301" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>0</v>
       </c>
@@ -11390,13 +11393,13 @@
         <v>4</v>
       </c>
       <c r="H302" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I302" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>0</v>
       </c>
@@ -11416,13 +11419,13 @@
         <v>4</v>
       </c>
       <c r="H303" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I303" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>0</v>
       </c>
@@ -11442,13 +11445,13 @@
         <v>4</v>
       </c>
       <c r="H304" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="I304" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>0</v>
       </c>
@@ -11468,19 +11471,19 @@
         <v>626</v>
       </c>
       <c r="H305" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="I305" t="s">
         <v>905</v>
       </c>
       <c r="K305" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L305" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>0</v>
       </c>
@@ -11500,19 +11503,19 @@
         <v>860</v>
       </c>
       <c r="H306" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="I306" t="s">
         <v>905</v>
       </c>
       <c r="K306" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L306" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>0</v>
       </c>
@@ -11532,19 +11535,19 @@
         <v>185</v>
       </c>
       <c r="H307" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="I307" t="s">
         <v>905</v>
       </c>
       <c r="K307" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L307" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>0</v>
       </c>
@@ -11564,7 +11567,7 @@
         <v>863</v>
       </c>
       <c r="H308" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I308" t="s">
         <v>905</v>
@@ -11573,7 +11576,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>0</v>
       </c>
@@ -11593,7 +11596,7 @@
         <v>769</v>
       </c>
       <c r="H309" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I309" t="s">
         <v>905</v>
@@ -11602,7 +11605,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>0</v>
       </c>
@@ -11622,7 +11625,7 @@
         <v>772</v>
       </c>
       <c r="H310" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I310" t="s">
         <v>905</v>
@@ -11631,7 +11634,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>0</v>
       </c>
@@ -11651,7 +11654,7 @@
         <v>775</v>
       </c>
       <c r="H311" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I311" t="s">
         <v>905</v>
@@ -11660,7 +11663,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>0</v>
       </c>
@@ -11680,7 +11683,7 @@
         <v>778</v>
       </c>
       <c r="H312" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I312" t="s">
         <v>905</v>
@@ -11689,7 +11692,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>0</v>
       </c>
@@ -11709,7 +11712,7 @@
         <v>781</v>
       </c>
       <c r="H313" t="s">
-        <v>1008</v>
+        <v>1021</v>
       </c>
       <c r="I313" t="s">
         <v>905</v>
@@ -11718,7 +11721,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>0</v>
       </c>
@@ -11738,13 +11741,13 @@
         <v>48</v>
       </c>
       <c r="H314" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="I314" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>0</v>
       </c>
@@ -11764,13 +11767,13 @@
         <v>591</v>
       </c>
       <c r="H315" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="I315" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>0</v>
       </c>
@@ -11790,13 +11793,13 @@
         <v>788</v>
       </c>
       <c r="H316" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="I316" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>0</v>
       </c>
@@ -11816,13 +11819,13 @@
         <v>791</v>
       </c>
       <c r="H317" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="I317" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>0</v>
       </c>
@@ -11842,13 +11845,13 @@
         <v>794</v>
       </c>
       <c r="H318" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="I318" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>0</v>
       </c>
@@ -11868,13 +11871,13 @@
         <v>797</v>
       </c>
       <c r="H319" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="I319" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>0</v>
       </c>
@@ -11894,13 +11897,13 @@
         <v>800</v>
       </c>
       <c r="H320" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="I320" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>0</v>
       </c>
@@ -11920,13 +11923,13 @@
         <v>133</v>
       </c>
       <c r="H321" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="I321" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>0</v>
       </c>
@@ -11946,13 +11949,13 @@
         <v>805</v>
       </c>
       <c r="H322" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="I322" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>0</v>
       </c>
@@ -11972,13 +11975,13 @@
         <v>591</v>
       </c>
       <c r="H323" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="I323" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>0</v>
       </c>
@@ -11998,13 +12001,13 @@
         <v>48</v>
       </c>
       <c r="H324" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="I324" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>0</v>
       </c>
@@ -12024,13 +12027,13 @@
         <v>810</v>
       </c>
       <c r="H325" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="I325" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>0</v>
       </c>
@@ -12050,13 +12053,13 @@
         <v>813</v>
       </c>
       <c r="H326" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="I326" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>0</v>
       </c>
@@ -12076,13 +12079,13 @@
         <v>185</v>
       </c>
       <c r="H327" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="I327" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>0</v>
       </c>
@@ -12102,13 +12105,13 @@
         <v>48</v>
       </c>
       <c r="H328" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="I328" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>0</v>
       </c>
@@ -12128,13 +12131,13 @@
         <v>817</v>
       </c>
       <c r="H329" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I329" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>0</v>
       </c>
@@ -12154,13 +12157,13 @@
         <v>818</v>
       </c>
       <c r="H330" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="I330" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>0</v>
       </c>
@@ -12180,13 +12183,13 @@
         <v>145</v>
       </c>
       <c r="H331" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I331" t="s">
         <v>1017</v>
       </c>
-      <c r="I331" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>0</v>
       </c>
@@ -12206,31 +12209,31 @@
         <v>820</v>
       </c>
       <c r="H332" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I332" t="s">
         <v>893</v>
       </c>
       <c r="K332" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="L332" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="M332" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="N332" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="O332" t="s">
+        <v>1014</v>
+      </c>
+      <c r="P332" t="s">
         <v>1017</v>
       </c>
-      <c r="P332" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>0</v>
       </c>
@@ -12250,13 +12253,13 @@
         <v>822</v>
       </c>
       <c r="H333" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="I333" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>0</v>
       </c>
@@ -12276,13 +12279,13 @@
         <v>824</v>
       </c>
       <c r="H334" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I334" t="s">
         <v>1017</v>
       </c>
-      <c r="I334" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>0</v>
       </c>
@@ -12302,13 +12305,13 @@
         <v>826</v>
       </c>
       <c r="H335" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="I335" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>0</v>
       </c>
@@ -12328,13 +12331,13 @@
         <v>828</v>
       </c>
       <c r="H336" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="I336" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>0</v>
       </c>
@@ -12354,13 +12357,13 @@
         <v>865</v>
       </c>
       <c r="H337" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="I337" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>0</v>
       </c>
@@ -12380,13 +12383,13 @@
         <v>830</v>
       </c>
       <c r="H338" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="I338" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>0</v>
       </c>
@@ -12406,13 +12409,13 @@
         <v>832</v>
       </c>
       <c r="H339" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="I339" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>0</v>
       </c>
@@ -12432,10 +12435,10 @@
         <v>834</v>
       </c>
       <c r="H340" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="I340" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>